<commit_message>
add model and confusion
</commit_message>
<xml_diff>
--- a/model/鼾声识别acc_pre_f1_recall.xlsx
+++ b/model/鼾声识别acc_pre_f1_recall.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9300"/>
+    <workbookView windowWidth="23040" windowHeight="8700"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="29">
   <si>
     <t>cnn</t>
   </si>
@@ -100,9 +100,6 @@
   </si>
   <si>
     <t>PLPs</t>
-  </si>
-  <si>
-    <t>nan</t>
   </si>
   <si>
     <t>s</t>
@@ -1072,7 +1069,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="P53" sqref="P53"/>
+      <selection pane="bottomLeft" activeCell="K74" sqref="K74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1182,8 +1179,6 @@
       <c r="N2" s="1">
         <v>98.28</v>
       </c>
-      <c r="O2"/>
-      <c r="P2"/>
       <c r="AB2" s="2"/>
     </row>
     <row r="3" spans="9:9">
@@ -1228,8 +1223,6 @@
       <c r="K5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L5"/>
-      <c r="M5"/>
       <c r="O5" s="2"/>
       <c r="AE5" s="2"/>
       <c r="AI5" s="2"/>
@@ -1269,8 +1262,6 @@
       <c r="K6" s="1">
         <v>96.83</v>
       </c>
-      <c r="L6"/>
-      <c r="M6"/>
       <c r="O6" s="2"/>
       <c r="AB6" s="2"/>
     </row>
@@ -1320,8 +1311,6 @@
       <c r="N8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O8"/>
-      <c r="P8"/>
       <c r="AB8" s="2"/>
       <c r="AE8" s="4"/>
       <c r="AF8" s="5"/>
@@ -3547,8 +3536,6 @@
       <c r="K17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L17"/>
-      <c r="M17"/>
       <c r="O17" s="2"/>
     </row>
     <row r="18" spans="1:15">
@@ -3585,8 +3572,6 @@
       <c r="K18" s="1">
         <v>96.08</v>
       </c>
-      <c r="L18"/>
-      <c r="M18"/>
       <c r="O18" s="2"/>
     </row>
     <row r="20" spans="1:14">
@@ -3807,8 +3792,6 @@
       <c r="K27" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L27"/>
-      <c r="M27"/>
       <c r="O27" s="2"/>
     </row>
     <row r="28" spans="1:15">
@@ -3845,8 +3828,6 @@
       <c r="K28" s="1">
         <v>96.96</v>
       </c>
-      <c r="L28"/>
-      <c r="M28"/>
       <c r="O28" s="2"/>
     </row>
     <row r="30" spans="1:14">
@@ -4059,8 +4040,6 @@
       <c r="K37" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L37"/>
-      <c r="M37"/>
       <c r="O37" s="2"/>
     </row>
     <row r="38" spans="1:15">
@@ -4097,8 +4076,6 @@
       <c r="K38" s="1">
         <v>92.4</v>
       </c>
-      <c r="L38"/>
-      <c r="M38"/>
       <c r="O38" s="2"/>
     </row>
     <row r="40" spans="1:14">
@@ -4311,8 +4288,6 @@
       <c r="K47" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L47"/>
-      <c r="M47"/>
       <c r="O47" s="2"/>
     </row>
     <row r="48" spans="1:15">
@@ -4349,8 +4324,6 @@
       <c r="K48" s="1">
         <v>97.04</v>
       </c>
-      <c r="L48"/>
-      <c r="M48"/>
       <c r="O48" s="2"/>
     </row>
     <row r="49" spans="7:7">
@@ -4568,8 +4541,6 @@
       <c r="K57" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L57"/>
-      <c r="M57"/>
       <c r="O57" s="2"/>
     </row>
     <row r="58" spans="1:15">
@@ -4606,8 +4577,6 @@
       <c r="K58" s="1">
         <v>93.63</v>
       </c>
-      <c r="L58"/>
-      <c r="M58"/>
       <c r="O58" s="2"/>
     </row>
     <row r="60" spans="1:14">
@@ -4778,14 +4747,14 @@
       <c r="K65" s="1">
         <v>68.73</v>
       </c>
-      <c r="L65" s="1" t="s">
-        <v>28</v>
+      <c r="L65" s="1">
+        <v>52.74</v>
       </c>
       <c r="M65" s="1">
         <v>66.29</v>
       </c>
-      <c r="N65" s="1" t="s">
-        <v>28</v>
+      <c r="N65" s="1">
+        <v>58.74</v>
       </c>
       <c r="O65" s="3"/>
       <c r="P65" s="3"/>
@@ -4873,14 +4842,14 @@
       <c r="H68" s="1">
         <v>59.9</v>
       </c>
-      <c r="I68" s="1" t="s">
-        <v>28</v>
+      <c r="I68" s="1">
+        <v>50.69</v>
       </c>
       <c r="J68" s="1">
         <v>54.73</v>
       </c>
-      <c r="K68" s="1" t="s">
-        <v>28</v>
+      <c r="K68" s="1">
+        <v>52.63</v>
       </c>
       <c r="L68" s="3"/>
       <c r="M68" s="3"/>
@@ -4986,21 +4955,21 @@
       <c r="K71" s="1">
         <v>68.7</v>
       </c>
-      <c r="L71" s="1" t="s">
-        <v>28</v>
+      <c r="L71" s="1">
+        <v>52.74</v>
       </c>
       <c r="M71" s="1">
         <v>66.29</v>
       </c>
-      <c r="N71" s="1" t="s">
-        <v>28</v>
+      <c r="N71" s="1">
+        <v>58.74</v>
       </c>
       <c r="O71" s="3"/>
       <c r="P71" s="3"/>
     </row>
     <row r="75" spans="16:16">
       <c r="P75" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>